<commit_message>
This is updated data
</commit_message>
<xml_diff>
--- a/src/test/java/com/OrangeHrm/TestData/user_data.xlsx
+++ b/src/test/java/com/OrangeHrm/TestData/user_data.xlsx
@@ -27,18 +27,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="2">
   <si>
     <t>standard_user</t>
   </si>
   <si>
     <t>secret_sauce</t>
-  </si>
-  <si>
-    <t>secre_sauce</t>
-  </si>
-  <si>
-    <t>secret_suce</t>
   </si>
 </sst>
 </file>
@@ -996,7 +990,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="C14 F12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.45" outlineLevelRow="4" outlineLevelCol="1"/>
@@ -1034,7 +1028,7 @@
         <v>0</v>
       </c>
       <c r="B4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1042,7 +1036,7 @@
         <v>0</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>